<commit_message>
added the lr table
</commit_message>
<xml_diff>
--- a/tabela_sintatica.xlsx
+++ b/tabela_sintatica.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo\Dropbox\unioeste-ciências-da-computação\4º ano\compiladores\CGVlang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C481A0-A556-4598-8E89-52BFC0109C67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A216C43-EA3D-45F8-B999-D150F06DE603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="ColumnTitle_1e616d1e492041b1bfa19fc84d2f8e3e" localSheetId="0">Plan1!$B$1</definedName>
+    <definedName name="RowTitle_c8703dd001de419d9f627fd402702ab0" localSheetId="0">Plan1!$A$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -703,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" topLeftCell="X9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE34" sqref="AE34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
the excel table expr part is done
</commit_message>
<xml_diff>
--- a/tabela_sintatica.xlsx
+++ b/tabela_sintatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo\Documents\codes\CGVlang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAD5017-F5E5-45A9-B7A5-B43796680829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C42138-873F-4F97-ACFA-22A39656FADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="108">
   <si>
     <t>type</t>
   </si>
@@ -235,84 +235,12 @@
     <t>ϵ</t>
   </si>
   <si>
-    <t>EXPR_LO_AND EXPR_LO_OR_REST</t>
-  </si>
-  <si>
-    <t>ortoken EXPR_LO_AND EXPR_LO_OR_REST</t>
-  </si>
-  <si>
     <t>ortoken</t>
   </si>
   <si>
     <t>andtoken</t>
   </si>
   <si>
-    <t>EXPR_COMP_GE EXPR_LO_AND_REST</t>
-  </si>
-  <si>
-    <t>andtoken EXPR_COMP_GE EXPR_LO_AND_REST</t>
-  </si>
-  <si>
-    <t>&gt;= EXPR_COMP_LE EXPR_COMP_GE_REST</t>
-  </si>
-  <si>
-    <t>&lt;= EXPR_COMP_G EXPR_COMP_LE_REST</t>
-  </si>
-  <si>
-    <t>&gt; EXPR_COMP_L EXPR_COMP_G_REST</t>
-  </si>
-  <si>
-    <t>&lt; EXPR_COMP_E EXPR_COMP_L_REST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> == EXPR_ARIT_AS EXPR_COMP_E_REST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + EXPR_ARIT_MD EXPR_ARIT_AS_REST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - EXPR_ARIT_MD EXPR_ARIT_AS_REST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> * EXPR_ARIT_EXP EXPR_ARIT_MD_REST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> / EXPR_ARIT_EXP EXPR_ARIT_MD_REST</t>
-  </si>
-  <si>
-    <t>EXPR_COMP_LE EXPR_COMP_GE_REST</t>
-  </si>
-  <si>
-    <t>EXPR_COMP_G EXPR_COMP_LE_REST</t>
-  </si>
-  <si>
-    <t>EXPR_COMP_L EXPR_COMP_G_REST</t>
-  </si>
-  <si>
-    <t>EXPR_COMP_E EXPR_COMP_L_REST</t>
-  </si>
-  <si>
-    <t>EXPR_ARIT_AS EXPR_COMP_E_REST</t>
-  </si>
-  <si>
-    <t>EXPR_ARIT_MD EXPR_ARIT_AS_REST</t>
-  </si>
-  <si>
-    <t>EXPR_ARIT_EXP EXPR_ARIT_MD_REST</t>
-  </si>
-  <si>
-    <t>EXPR_NOT EXPR_ARIT_EXP_REST</t>
-  </si>
-  <si>
-    <t>~ EXPR_NOT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ** EXPR_ARIT_EXP</t>
-  </si>
-  <si>
-    <t>id EXPR_FINAL_REST</t>
-  </si>
-  <si>
     <t xml:space="preserve"> = EXPR</t>
   </si>
   <si>
@@ -331,13 +259,100 @@
     <t>( id , EXPR , EXPR , EXPR ) { S }</t>
   </si>
   <si>
-    <t>id TYPEDECL_ATTRIB | adiciona na tabela e gera declaração no código sem atribuição</t>
-  </si>
-  <si>
     <t>( id ) | get_rule</t>
   </si>
   <si>
     <t>type TYPEDECL S | set_type</t>
+  </si>
+  <si>
+    <t>ϵ | end_scope</t>
+  </si>
+  <si>
+    <t>id TYPEDECL_ATTRIB | add_symbol</t>
+  </si>
+  <si>
+    <t>EXPR_LO_AND EXPR_LO_OR_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_COMP_GE EXPR_LO_AND_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_COMP_GE EXPR_LO_AND_REST  | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_COMP_LE EXPR_COMP_GE_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_COMP_G EXPR_COMP_LE_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_COMP_L EXPR_COMP_G_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_COMP_E EXPR_COMP_L_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_ARIT_AS EXPR_COMP_E_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_ARIT_MD EXPR_ARIT_AS_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_ARIT_EXP EXPR_ARIT_MD_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>EXPR_NOT EXPR_ARIT_EXP_REST | expr_move_down_rule</t>
+  </si>
+  <si>
+    <t>~ EXPR_NOT  | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * EXPR_ARIT_EXP EXPR_ARIT_MD_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> / EXPR_ARIT_EXP EXPR_ARIT_MD_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + EXPR_ARIT_MD EXPR_ARIT_AS_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - EXPR_ARIT_MD EXPR_ARIT_AS_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> == EXPR_ARIT_AS EXPR_COMP_E_REST  | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>andtoken EXPR_COMP_GE EXPR_LO_AND_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>ortoken EXPR_LO_AND EXPR_LO_OR_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>&gt;= EXPR_COMP_LE EXPR_COMP_GE_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>&lt;= EXPR_COMP_G EXPR_COMP_LE_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>&gt; EXPR_COMP_L EXPR_COMP_G_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>&lt; EXPR_COMP_E EXPR_COMP_L_REST | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ** EXPR_ARIT_EXP | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>ϵ | expr_move_up_rule</t>
+  </si>
+  <si>
+    <t>val | expr_set_operand_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = EXPR | expr_set_operator_rule</t>
+  </si>
+  <si>
+    <t>id EXPR_FINAL_REST | expr_set_operand_rule</t>
   </si>
 </sst>
 </file>
@@ -409,7 +424,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -424,6 +439,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,10 +789,10 @@
         <v>58</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>6</v>
@@ -842,7 +860,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>61</v>
@@ -887,7 +905,7 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="2" t="s">
@@ -1040,16 +1058,16 @@
         <v>59</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>59</v>
@@ -1071,85 +1089,85 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -1212,16 +1230,16 @@
         <v>59</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="Y6" s="5" t="s">
         <v>59</v>
@@ -1243,85 +1261,85 @@
         <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1415,85 +1433,85 @@
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -1587,85 +1605,85 @@
         <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -1736,7 +1754,7 @@
       <c r="W12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="X12" s="5" t="s">
+      <c r="X12" s="6" t="s">
         <v>85</v>
       </c>
       <c r="Y12" s="5" t="s">
@@ -1759,85 +1777,85 @@
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -1908,7 +1926,7 @@
       <c r="W14" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="X14" s="5" t="s">
+      <c r="X14" s="6" t="s">
         <v>86</v>
       </c>
       <c r="Y14" s="5" t="s">
@@ -1931,85 +1949,85 @@
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2103,85 +2121,85 @@
         <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
@@ -2275,85 +2293,85 @@
         <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
@@ -2447,85 +2465,85 @@
         <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
@@ -2619,85 +2637,85 @@
         <v>57</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AC23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
@@ -2849,13 +2867,13 @@
         <v>59</v>
       </c>
       <c r="V25" s="5" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="X25" s="5" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>59</v>
@@ -2947,7 +2965,7 @@
         <v>67</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2" t="s">
@@ -3002,7 +3020,7 @@
         <v>59</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="X27" s="5" t="s">
         <v>59</v>
@@ -3073,7 +3091,7 @@
         <v>59</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2" t="s">
@@ -3129,7 +3147,7 @@
         <v>59</v>
       </c>
       <c r="X29" s="5" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="Y29" s="5" t="s">
         <v>59</v>
@@ -3189,7 +3207,7 @@
         <v>59</v>
       </c>
       <c r="X30" s="5" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="Y30" s="5" t="s">
         <v>59</v>
@@ -3249,7 +3267,7 @@
         <v>59</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="Y31" s="5" t="s">
         <v>59</v>
@@ -3287,7 +3305,7 @@
         <v>67</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -3371,7 +3389,7 @@
         <v>59</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="Y33" s="5" t="s">
         <v>59</v>
@@ -3431,7 +3449,7 @@
         <v>59</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="Y34" s="5" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
re save the excel table
</commit_message>
<xml_diff>
--- a/tabela_sintatica.xlsx
+++ b/tabela_sintatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo\Documents\codes\CGVlang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8662DA6B-16F3-4D81-A4B7-B4ABADDA0FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44F9E0C-53AA-41F0-BFC0-C1AF21CBBB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed useless casts, and added the typedecl with = expr
</commit_message>
<xml_diff>
--- a/tabela_sintatica.xlsx
+++ b/tabela_sintatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo\Documents\codes\CGVlang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44F9E0C-53AA-41F0-BFC0-C1AF21CBBB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCBABED-EE79-443E-A563-9B18538189C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="109">
   <si>
     <t>type</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>id EXPR_FINAL_REST | expr_set_operand_rule</t>
+  </si>
+  <si>
+    <t>ϵ | demand_action_rule</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,9 +442,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z26" sqref="Z26"/>
+    <sheetView tabSelected="1" topLeftCell="X2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1754,7 @@
       <c r="W12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="X12" s="6" t="s">
+      <c r="X12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="Y12" s="5" t="s">
@@ -1926,7 +1926,7 @@
       <c r="W14" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="X14" s="6" t="s">
+      <c r="X14" s="2" t="s">
         <v>86</v>
       </c>
       <c r="Y14" s="5" t="s">
@@ -3045,22 +3045,22 @@
         <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -3076,16 +3076,16 @@
       <c r="S28" s="2"/>
       <c r="T28" s="5"/>
       <c r="U28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="Y28" s="5" t="s">
         <v>59</v>
@@ -3095,11 +3095,11 @@
       </c>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="AC28" s="5"/>
       <c r="AD28" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added the doif rules
</commit_message>
<xml_diff>
--- a/tabela_sintatica.xlsx
+++ b/tabela_sintatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo\Documents\codes\CGVlang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2730DC-789B-4827-AAEA-FBC736F1515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288DB31D-8C45-4551-BBBD-438E19B914D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,12 +247,6 @@
     <t>( EXPR )</t>
   </si>
   <si>
-    <t>maybe_not { S }</t>
-  </si>
-  <si>
-    <t>( EXPR ) { S } MAYBE_NOT</t>
-  </si>
-  <si>
     <t>( EXPR ) { S }</t>
   </si>
   <si>
@@ -359,6 +353,12 @@
   </si>
   <si>
     <t>( EXPR ) | put_rule</t>
+  </si>
+  <si>
+    <t>( EXPR ) { S } MAYBE_NOT | do_if_rule</t>
+  </si>
+  <si>
+    <t>maybe_not { S } | maybe_not_rule</t>
   </si>
 </sst>
 </file>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>61</v>
@@ -908,7 +908,7 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="2" t="s">
@@ -1061,16 +1061,16 @@
         <v>59</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>59</v>
@@ -1092,85 +1092,85 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -1233,16 +1233,16 @@
         <v>59</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Y6" s="5" t="s">
         <v>59</v>
@@ -1264,85 +1264,85 @@
         <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1405,16 +1405,16 @@
         <v>59</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>59</v>
@@ -1436,85 +1436,85 @@
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -1577,16 +1577,16 @@
         <v>59</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Y10" s="5" t="s">
         <v>59</v>
@@ -1608,85 +1608,85 @@
         <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -1749,16 +1749,16 @@
         <v>59</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>59</v>
@@ -1780,85 +1780,85 @@
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -1921,16 +1921,16 @@
         <v>59</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Y14" s="5" t="s">
         <v>59</v>
@@ -1952,85 +1952,85 @@
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2093,16 +2093,16 @@
         <v>59</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Y16" s="5" t="s">
         <v>59</v>
@@ -2124,85 +2124,85 @@
         <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
@@ -2265,16 +2265,16 @@
         <v>59</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Y18" s="5" t="s">
         <v>59</v>
@@ -2296,85 +2296,85 @@
         <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
@@ -2437,16 +2437,16 @@
         <v>59</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>59</v>
@@ -2468,85 +2468,85 @@
         <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
@@ -2609,16 +2609,16 @@
         <v>59</v>
       </c>
       <c r="U22" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="V22" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="X22" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Y22" s="5" t="s">
         <v>59</v>
@@ -2640,85 +2640,85 @@
         <v>57</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
@@ -2781,7 +2781,7 @@
         <v>59</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V24" s="2" t="s">
         <v>47</v>
@@ -2870,10 +2870,10 @@
         <v>59</v>
       </c>
       <c r="V25" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="W25" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="W25" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="X25" s="5" t="s">
         <v>71</v>
@@ -2968,7 +2968,7 @@
         <v>67</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2" t="s">
@@ -3023,7 +3023,7 @@
         <v>59</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="X27" s="5" t="s">
         <v>59</v>
@@ -3048,22 +3048,22 @@
         <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -3079,16 +3079,16 @@
       <c r="S28" s="2"/>
       <c r="T28" s="5"/>
       <c r="U28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Y28" s="5" t="s">
         <v>59</v>
@@ -3098,11 +3098,11 @@
       </c>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AC28" s="5"/>
       <c r="AD28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
@@ -3150,7 +3150,7 @@
         <v>59</v>
       </c>
       <c r="X29" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Y29" s="5" t="s">
         <v>59</v>
@@ -3210,7 +3210,7 @@
         <v>59</v>
       </c>
       <c r="X30" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Y30" s="5" t="s">
         <v>59</v>
@@ -3270,7 +3270,7 @@
         <v>59</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="Y31" s="5" t="s">
         <v>59</v>
@@ -3290,25 +3290,25 @@
         <v>53</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -3323,28 +3323,28 @@
       <c r="S32" s="2"/>
       <c r="T32" s="5"/>
       <c r="U32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AC32" s="5"/>
       <c r="AD32" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>59</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Y33" s="5" t="s">
         <v>59</v>
@@ -3452,7 +3452,7 @@
         <v>59</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Y34" s="5" t="s">
         <v>59</v>

</xml_diff>